<commit_message>
EE-1836-added choices and joint input file
For further information go to: https://www.ebi.ac.uk/panda/jira/browse/EE-1836?focusedCommentId=354286&page=com.atlassian.jira.plugin.system.issuetabpanels%3Acomment-tabpanel#comment-354286
</commit_message>
<xml_diff>
--- a/templates/sequence-based-metadata/study_template.xlsx
+++ b/templates/sequence-based-metadata/study_template.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-repositories\ega-metadata-schema\templates\sequence-based-metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcasado\Documents\GitHub\ega-metadata-schema\templates\sequence-based-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EA1CE9-2B62-4990-B278-1F95443F83D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A844155-7D7B-4F87-846C-D26ECF483EC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="study" sheetId="1" r:id="rId1"/>
+    <sheet name="Readme" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,19 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
-  <si>
-    <t>Center_name</t>
-  </si>
-  <si>
-    <t>TODO: ACCOUNT CENTER_NAME ACRONYM</t>
-  </si>
-  <si>
-    <t>Study_alias</t>
-  </si>
-  <si>
-    <t>TODO: UNIQUE NAME FOR STUDY</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
   <si>
     <t>Tag</t>
   </si>
@@ -48,22 +37,140 @@
     <t>Units</t>
   </si>
   <si>
-    <t>TODO: TAG VALUE</t>
-  </si>
-  <si>
-    <t>TODO: OPTIONAL UNIT</t>
-  </si>
-  <si>
-    <t>TODO: STUDY TITLE AS IT COULD APPEAR IN A PUBLICATION</t>
-  </si>
-  <si>
-    <t>Study_title</t>
-  </si>
-  <si>
-    <t>Existing_study_type</t>
-  </si>
-  <si>
-    <t>TODO: CONTROLLED VOCABULARY for study type: 
+    <t>Broker_name</t>
+  </si>
+  <si>
+    <t>Center_name*</t>
+  </si>
+  <si>
+    <t>Study_alias*</t>
+  </si>
+  <si>
+    <t>Study_title*</t>
+  </si>
+  <si>
+    <t>New_study_type</t>
+  </si>
+  <si>
+    <t>Existing_study_type*</t>
+  </si>
+  <si>
+    <t>Study_abstract</t>
+  </si>
+  <si>
+    <t>Center_ProjectName</t>
+  </si>
+  <si>
+    <t>RelatedStudy_DB</t>
+  </si>
+  <si>
+    <t>RelatedStudy_ID</t>
+  </si>
+  <si>
+    <t>RelatedStudy_label</t>
+  </si>
+  <si>
+    <t>RelatedStudy_IsPrimary</t>
+  </si>
+  <si>
+    <t>Study_description</t>
+  </si>
+  <si>
+    <t>TODO: More extensive free-form description of the study.</t>
+  </si>
+  <si>
+    <t>TODO: Name of the custom attribute.</t>
+  </si>
+  <si>
+    <t>TODO: Value of the custom attribute.</t>
+  </si>
+  <si>
+    <t>TODO: Optional scientific units.</t>
+  </si>
+  <si>
+    <t>EBI-TEST</t>
+  </si>
+  <si>
+    <t>EGA</t>
+  </si>
+  <si>
+    <t>Whole Genome Sequencing</t>
+  </si>
+  <si>
+    <t>Absiella dolichum DSM 3991</t>
+  </si>
+  <si>
+    <t>A pilot study examining genetic determinants associated with long term memory acquisition using exome sequencing of individuals from the outskirts of London.</t>
+  </si>
+  <si>
+    <t>PROJECT</t>
+  </si>
+  <si>
+    <t>PRJNA89519</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>bioproject</t>
+  </si>
+  <si>
+    <t>PRJNA110649</t>
+  </si>
+  <si>
+    <t>Project Contributor</t>
+  </si>
+  <si>
+    <t>UniEuk_EukBank</t>
+  </si>
+  <si>
+    <t>study keyword</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>TODO: The center name (its acronym) of the submitter's account (e.g. EBI-TEST)</t>
+  </si>
+  <si>
+    <t>TODO: The center name (its acronym) of the broker (e.g. EGA)</t>
+  </si>
+  <si>
+    <t>TODO: Title (free-form string) of the study as would be used in a publication</t>
+  </si>
+  <si>
+    <t>TODO: Study abstract (free-form string) as it could appear in a publication. Briefly describes the goals, purpose, and scope of the Study.  This does not need to be listed if it can be inherited from a referenced publication.</t>
+  </si>
+  <si>
+    <t>TODO: Submitter defined project name (e.g. 'Absiella dolichum DSM 3991').  This field is intended for backward tracking of the study record to the submitter's LIMS.</t>
+  </si>
+  <si>
+    <t>TODO: Submitter designated name for the 'Study' (e.g. 'My_study_HumanMicrobiome'). The name must be unique within the submission account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO: In case the overall purpose of the Study cannot be found in the existing types list, you may propose a new term. To do so, you shall use 'Other' as Existing_study_type, and enter here a new study type. Otherwise, leave this column empty. </t>
+  </si>
+  <si>
+    <t>TODO: Database of the related study (e.g. 'bioproject'). This value has to match with the NCBI controlled vocabulary of permitted cross references (see list: http://www.ncbi.nlm.nih.gov/entrez/eutils/einfo.fcgi?)
+If there are several related studies, you may repeat the block 'RelatedStudy_DB' - 'RelatedStudy_ID' - 'RelatedStudy_label' - 'RelatedStudy_IsPrimary'</t>
+  </si>
+  <si>
+    <t>TODO: Numeric record ID of the related Study (e.g. 406), meaningful to the NCBI Entrez system.
+If there are several related studies, you may repeat the block 'RelatedStudy_DB' - 'RelatedStudy_ID' - 'RelatedStudy_label' - 'RelatedStudy_IsPrimary'</t>
+  </si>
+  <si>
+    <t>TODO: How to label the link to the related Study (e.g. PRJNA89519).
+If there are several related studies, you may repeat the block 'RelatedStudy_DB' - 'RelatedStudy_ID' - 'RelatedStudy_label' - 'RelatedStudy_IsPrimary'</t>
+  </si>
+  <si>
+    <t>TODO: Whether this study object is designated as the primary source of the study or project information (use 'true' or 'false').
+If there are several related studies, you may repeat the block 'RelatedStudy_DB' - 'RelatedStudy_ID' - 'RelatedStudy_label' - 'RelatedStudy_IsPrimary'</t>
+  </si>
+  <si>
+    <t>TODO: Overall purpose of the study. Must be value from Controlled vocabulary: 
     Whole Genome Sequencing
     Metagenomics
     Transcriptome Analysis
@@ -81,20 +188,123 @@
     Other (Study type not listed)</t>
   </si>
   <si>
-    <t>TODO: STUDY ABSTRACT AS IT COULD APPEAR IN A PUBLICATION</t>
-  </si>
-  <si>
-    <t>Study_abstract</t>
-  </si>
-  <si>
-    <t>TODO: TAG NAME</t>
+    <t>Lastname, Firstname</t>
+  </si>
+  <si>
+    <t>Example!_Human Microbiome Project SP56J</t>
+  </si>
+  <si>
+    <t>Example!_Strain for comparative analysis</t>
+  </si>
+  <si>
+    <t>Example!_Background: In 2013, a prospective registry for adults with congenital heart disease (CHD) was established in Switzerland, providing detailed data on disease characteristics and outcomes: Swiss Adult Congenital HEart disease Registry (SACHER). Its aim is to improve the knowledge base of outcomes in adults with CHD. The registry design and baseline patient characteristics are reported.
+Methods: All patients with structural congenital heart defects or hereditary aortopathies, followed-up at dedicated adult CHD clinics, are asked to participate in SACHER. Data of participants are pseudonymised and collected in an electronic, web-based, database (secuTrial®). Collected data include detailed diagnosis, type of repair procedures, previous complications and adverse outcomes during follow-up.
+Results: From May 2014 to December 2016, 2836 patients (54% male, mean age 34 ± 14 years), with a wide variety of congenital heart lesions, have been enrolled into SACHER. Most prevalent were valve lesions (25%), followed by shunt lesions (22%), cyanotic and other complex congenital heart disease (16%), diseases affecting the right heart, i.e., tetralogy of Fallot or Ebstein anomaly (15%), and diseases of the left ventricular outflow tract (13%); 337 patients (12%) had concomitant congenital syndromes. The majority had undergone previous repair procedures (71%), 47% of those had one or more reinterventions.
+Conclusion: SACHER collects multicentre data on adults with CHD. Its structure enables prospective data analysis to assess detailed, lesion-specific outcomes with the aim to finally improve long-term outcomes.</t>
+  </si>
+  <si>
+    <t>Provide your real metadata below this row (each row under this one will account for one metadata instance)</t>
+  </si>
+  <si>
+    <t>Rows format</t>
+  </si>
+  <si>
+    <t>Row number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Column headers</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descriptive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> row (explains what type of data corresponds to each column)</t>
+    </r>
+  </si>
+  <si>
+    <t>Real data ceiling (put your real data beneath this row)</t>
+  </si>
+  <si>
+    <t>4 onwards</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Real data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (all rows from 4 onwards will be transformed into XMLs)</t>
+    </r>
+  </si>
+  <si>
+    <t>Column headers' colour format</t>
+  </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>Bright yellow</t>
+  </si>
+  <si>
+    <t>Required attributes</t>
+  </si>
+  <si>
+    <t>No colour</t>
+  </si>
+  <si>
+    <t>Optional (highly recommended) attributes</t>
+  </si>
+  <si>
+    <t>Dark grey</t>
+  </si>
+  <si>
+    <t>Ignore this column (based on multiple choice attributes)</t>
+  </si>
+  <si>
+    <t>Other colours</t>
+  </si>
+  <si>
+    <t>Repeated blocks (each with their own colour): you can add or remove as many "whole" blocks as you want to fulfil your needs, but remember to always work with complete repetitions (e.g. TAG-VALUE-UNITS columns for an attribute)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,8 +312,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,7 +345,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -124,18 +369,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -144,7 +407,55 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -156,23 +467,174 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -448,102 +910,428 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="1" customWidth="1"/>
+    <col min="6" max="9" width="15.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="24" customWidth="1"/>
+    <col min="11" max="12" width="8.7109375" style="3" customWidth="1"/>
+    <col min="13" max="15" width="8.7109375" style="20" customWidth="1"/>
+    <col min="16" max="18" width="8.7109375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" style="6" customWidth="1"/>
+    <col min="20" max="22" width="10.85546875" style="8" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" style="20" customWidth="1"/>
+    <col min="24" max="26" width="10.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="M1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="N1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="T1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="V1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="W1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="Y1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="Z1" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z2" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="36" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="37"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+    </row>
+    <row r="4" spans="1:26" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="18"/>
+      <c r="P4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" s="12"/>
+      <c r="S4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="14">
+        <v>406</v>
+      </c>
+      <c r="U4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" s="11">
+        <v>110649</v>
+      </c>
+      <c r="Y4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z4" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:I1 K1:L1 T1:V1 AA1:XFD1">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="~*">
+      <formula>NOT(ISERROR(SEARCH("~*",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="~*">
+      <formula>NOT(ISERROR(SEARCH("~*",S1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X1:Z1">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="~*">
+      <formula>NOT(ISERROR(SEARCH("~*",X1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W1">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="~*">
+      <formula>NOT(ISERROR(SEARCH("~*",W1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1:O1">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="~*">
+      <formula>NOT(ISERROR(SEARCH("~*",N1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1:R1">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="~*">
+      <formula>NOT(ISERROR(SEARCH("~*",Q1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00CCDD5A-D5FA-4FC3-BA6B-CA2A01EC7C7B}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="40"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="40"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A9:B9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>